<commit_message>
Database and effect ID reference
- SQLite database
- Effect ID reference Excel sheet
</commit_message>
<xml_diff>
--- a/Content/Database/EffectIDReference.xlsx
+++ b/Content/Database/EffectIDReference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Num:</t>
   </si>
@@ -72,6 +72,48 @@
   </si>
   <si>
     <t>Aegis</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Bounce Heal</t>
+  </si>
+  <si>
+    <t>Unnamed AOE Bubble</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Chloroplast</t>
+  </si>
+  <si>
+    <t>Nature's Touch</t>
+  </si>
+  <si>
+    <t>Replenishing Winds</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove Aura</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove HOT</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove Ref</t>
+  </si>
+  <si>
+    <t>Replenish</t>
+  </si>
+  <si>
+    <t>Living Seed</t>
+  </si>
+  <si>
+    <t>Hibernate Friend</t>
+  </si>
+  <si>
+    <t>Hibernate Foe</t>
   </si>
 </sst>
 </file>
@@ -392,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,6 +566,118 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Database and effect ID reference"
This reverts commit f47bb01819c42ee45bc215cc72517ddf6be17974.
</commit_message>
<xml_diff>
--- a/Content/Database/EffectIDReference.xlsx
+++ b/Content/Database/EffectIDReference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Num:</t>
   </si>
@@ -72,48 +72,6 @@
   </si>
   <si>
     <t>Aegis</t>
-  </si>
-  <si>
-    <t>Shield</t>
-  </si>
-  <si>
-    <t>Bounce Heal</t>
-  </si>
-  <si>
-    <t>Unnamed AOE Bubble</t>
-  </si>
-  <si>
-    <t>Regeneration</t>
-  </si>
-  <si>
-    <t>Chloroplast</t>
-  </si>
-  <si>
-    <t>Nature's Touch</t>
-  </si>
-  <si>
-    <t>Replenishing Winds</t>
-  </si>
-  <si>
-    <t>Blessing of the Grove Aura</t>
-  </si>
-  <si>
-    <t>Blessing of the Grove HOT</t>
-  </si>
-  <si>
-    <t>Blessing of the Grove Ref</t>
-  </si>
-  <si>
-    <t>Replenish</t>
-  </si>
-  <si>
-    <t>Living Seed</t>
-  </si>
-  <si>
-    <t>Hibernate Friend</t>
-  </si>
-  <si>
-    <t>Hibernate Foe</t>
   </si>
 </sst>
 </file>
@@ -434,16 +392,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -566,118 +524,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Database and effect ID reference""
This reverts commit 4abf39120b851504078d84eccbaf0930c1c7d2f8.
</commit_message>
<xml_diff>
--- a/Content/Database/EffectIDReference.xlsx
+++ b/Content/Database/EffectIDReference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Num:</t>
   </si>
@@ -72,6 +72,48 @@
   </si>
   <si>
     <t>Aegis</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Bounce Heal</t>
+  </si>
+  <si>
+    <t>Unnamed AOE Bubble</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Chloroplast</t>
+  </si>
+  <si>
+    <t>Nature's Touch</t>
+  </si>
+  <si>
+    <t>Replenishing Winds</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove Aura</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove HOT</t>
+  </si>
+  <si>
+    <t>Blessing of the Grove Ref</t>
+  </si>
+  <si>
+    <t>Replenish</t>
+  </si>
+  <si>
+    <t>Living Seed</t>
+  </si>
+  <si>
+    <t>Hibernate Friend</t>
+  </si>
+  <si>
+    <t>Hibernate Foe</t>
   </si>
 </sst>
 </file>
@@ -392,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,6 +566,118 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>